<commit_message>
Updated description of problems on activities
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\ConcurrencyEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5A9066-3C48-446C-AA48-F7F73D0D8853}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EF806B-B527-4A1A-A79B-4845A9BD0B86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7665" yWindow="4545" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Previsão para completar</t>
   </si>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +472,9 @@
       <c r="B8" s="1">
         <v>43688</v>
       </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
Extended matrix multiplication implementations to support any size and any number of tasks
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\ConcurrencyEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EF806B-B527-4A1A-A79B-4845A9BD0B86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0BA7CC-D9B9-48A5-B84D-6AC7220575B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7665" yWindow="4545" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Previsão para completar</t>
   </si>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,6 +483,9 @@
       <c r="B9" s="1">
         <v>43688</v>
       </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
Extended concurrent sum implementations to support any amount of numbers and any number of tasks
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\ConcurrencyEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0BA7CC-D9B9-48A5-B84D-6AC7220575B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78BE027-FFB7-4C59-AD71-6B84E5274BB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2880" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Previsão para completar</t>
   </si>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +459,9 @@
       <c r="B6" s="1">
         <v>43687</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">

</xml_diff>

<commit_message>
Refactor layouts and values of download problem to the download of an image of user choose
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\ConcurrencyEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78BE027-FFB7-4C59-AD71-6B84E5274BB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4C9BED-AECA-4520-A394-298A0B3A56BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2880" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Previsão para completar</t>
   </si>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +443,9 @@
       <c r="B4" s="1">
         <v>43683</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>